<commit_message>
Updated dashboard portfolio and added lots of to be modeled spreadsheets
</commit_message>
<xml_diff>
--- a/Consumer/Chipotle Mexican Grill.xlsx
+++ b/Consumer/Chipotle Mexican Grill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Consumer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1399E4-7432-BD48-879B-97D2A0213F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28D03C6-CC8D-6840-B5F8-2E14BE4C0883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5540" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -2378,9 +2378,9 @@
     <v>Powered by Refinitiv</v>
     <v>2139.88</v>
     <v>1233.6099999999999</v>
-    <v>1.3165</v>
-    <v>-8.3000000000000007</v>
-    <v>-4.0479999999999995E-3</v>
+    <v>1.3229</v>
+    <v>9.11</v>
+    <v>4.3350000000000003E-3</v>
     <v>USD</v>
     <v>Chipotle Mexican Grill, Inc., together with its subsidiaries, owns and operates Chipotle Mexican Grill restaurants. The Company’s Chipotle Mexican Grill restaurants serve a relevant menu of burritos, burrito bowls (a burrito without the tortilla), quesadillas, tacos, and salads. The Company has approximately 3,200 restaurants in the United States, Canada, the United Kingdom, France and Germany. The Company manages its operations based on eight regions. It sells gift cards, which do not have expiration dates. In its Chipotle restaurants, the Company serves only meats and brands these meats as Responsibly Raised. The Company’s subsidiaries include Chipotle Mexican Grill Canada Corp., Chipotle Mexican Grill France SAS, Chipotle Mexican Grill Germany GMBH, Chipotle Mexican Grill of Berwyn Heights, LLC, Chipotle Mexican Grill of Colorado, LLC, Chipotle Mexican Grill of Kansas, LLC, Chipotle Mexican Grill of Maryland, LLC, SP Kitchens, LLC and Chipotle Mexican Grill Texas Holdings, LLC.</v>
     <v>104958</v>
@@ -2388,24 +2388,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>610 Newport Center Dr, Suite 1100, NEWPORT BEACH, CA, 92660 US</v>
-    <v>2059.09</v>
+    <v>2124.9899999999998</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45100.783510925779</v>
+    <v>45106.996204050782</v>
     <v>0</v>
-    <v>2037.76</v>
-    <v>56344523044</v>
+    <v>2102.8850000000002</v>
+    <v>58231116304</v>
     <v>CHIPOTLE MEXICAN GRILL, INC.</v>
     <v>CHIPOTLE MEXICAN GRILL, INC.</v>
-    <v>2048</v>
-    <v>55.471299999999999</v>
-    <v>2050.52</v>
-    <v>2042.22</v>
+    <v>2103.27</v>
+    <v>57.096600000000002</v>
+    <v>2101.4899999999998</v>
+    <v>2110.6</v>
     <v>27589840</v>
     <v>CMG</v>
     <v>CHIPOTLE MEXICAN GRILL, INC. (XNYS:CMG)</v>
-    <v>146543</v>
-    <v>265706</v>
+    <v>2</v>
+    <v>276575</v>
     <v>1998</v>
   </rv>
   <rv s="2">
@@ -2558,10 +2558,10 @@
       <v>4</v>
     </spb>
     <spb s="4">
-      <v>Real-Time Nasdaq Last Sale</v>
+      <v>Delayed 15 minutes</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
+      <v>Source: Nasdaq</v>
       <v>GMT</v>
     </spb>
   </spbData>
@@ -2978,7 +2978,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="S89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X98" sqref="X98"/>
+      <selection pane="bottomRight" activeCell="Z104" sqref="Z104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4381,15 +4381,15 @@
       </c>
       <c r="AD16" s="30">
         <f>AE101/W3</f>
-        <v>6.5253959330381814</v>
+        <v>6.7438868762748054</v>
       </c>
       <c r="AE16" s="30">
         <f>AE101/W28</f>
-        <v>62.667623597348907</v>
+        <v>64.765934309938487</v>
       </c>
       <c r="AF16" s="31">
         <f>AE101/W106</f>
-        <v>66.757727106745733</v>
+        <v>68.992987451644822</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -10187,7 +10187,7 @@
       </c>
       <c r="AE95" s="56" cm="1">
         <f t="array" ref="AE95">_FV(A1,"Beta")</f>
-        <v>1.3165</v>
+        <v>1.3229</v>
       </c>
     </row>
     <row r="96" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10342,7 +10342,7 @@
       </c>
       <c r="AE97" s="35">
         <f>(AE94)+((AE95)*(AE96-AE94))</f>
-        <v>9.7625325000000013E-2</v>
+        <v>9.7900845000000014E-2</v>
       </c>
     </row>
     <row r="98" spans="1:31" ht="19" x14ac:dyDescent="0.25">
@@ -10573,7 +10573,7 @@
       </c>
       <c r="AE100" s="33">
         <f>AE99/AE103</f>
-        <v>6.2111561334671092E-2</v>
+        <v>6.0220430356454309E-2</v>
       </c>
     </row>
     <row r="101" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10651,7 +10651,7 @@
       </c>
       <c r="AE101" s="48" cm="1">
         <f t="array" ref="AE101">_FV(A1,"Market cap",TRUE)</f>
-        <v>56344523044</v>
+        <v>58231116304</v>
       </c>
     </row>
     <row r="102" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10729,7 +10729,7 @@
       </c>
       <c r="AE102" s="33">
         <f>AE101/AE103</f>
-        <v>0.93788843866532889</v>
+        <v>0.9397795696435457</v>
       </c>
     </row>
     <row r="103" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -10807,7 +10807,7 @@
       </c>
       <c r="AE103" s="37">
         <f>AE99+AE101</f>
-        <v>60075933044</v>
+        <v>61962526304</v>
       </c>
     </row>
     <row r="104" spans="1:31" ht="19" x14ac:dyDescent="0.25">
@@ -10985,7 +10985,7 @@
       </c>
       <c r="AE105" s="26">
         <f>(AE100*AE92)+(AE102*AE97)</f>
-        <v>9.1829285275850228E-2</v>
+        <v>9.226468725591136E-2</v>
       </c>
     </row>
     <row r="106" spans="1:31" ht="19" x14ac:dyDescent="0.25">
@@ -11119,7 +11119,7 @@
       <c r="AA107" s="38"/>
       <c r="AB107" s="41">
         <f>AB106*(1+AE107)/(AE108-AE107)</f>
-        <v>24387343527.096115</v>
+        <v>24229485101.02879</v>
       </c>
       <c r="AC107" s="42" t="s">
         <v>147</v>
@@ -11150,7 +11150,7 @@
       </c>
       <c r="AB108" s="41">
         <f>AB107+AB106</f>
-        <v>25977381319.966812</v>
+        <v>25819522893.899487</v>
       </c>
       <c r="AC108" s="42" t="s">
         <v>143</v>
@@ -11160,7 +11160,7 @@
       </c>
       <c r="AE108" s="46">
         <f>AE105</f>
-        <v>9.1829285275850228E-2</v>
+        <v>9.226468725591136E-2</v>
       </c>
     </row>
     <row r="109" spans="1:31" ht="19" x14ac:dyDescent="0.25">
@@ -11175,7 +11175,7 @@
       </c>
       <c r="Y110" s="48">
         <f>NPV(AE108,X108,Y108,Z108,AA108,AB108)</f>
-        <v>20466133549.864021</v>
+        <v>20327471157.908424</v>
       </c>
     </row>
     <row r="111" spans="1:31" ht="20" x14ac:dyDescent="0.25">
@@ -11202,7 +11202,7 @@
       </c>
       <c r="Y113" s="48">
         <f>Y110+Y111-Y112</f>
-        <v>17633859549.864021</v>
+        <v>17495197157.908424</v>
       </c>
     </row>
     <row r="114" spans="24:25" ht="20" x14ac:dyDescent="0.25">
@@ -11220,7 +11220,7 @@
       </c>
       <c r="Y115" s="51">
         <f>Y113/Y114</f>
-        <v>639.41601446045956</v>
+        <v>634.38801966617837</v>
       </c>
     </row>
     <row r="116" spans="24:25" ht="20" x14ac:dyDescent="0.25">
@@ -11229,7 +11229,7 @@
       </c>
       <c r="Y116" s="58" cm="1">
         <f t="array" ref="Y116">_FV(A1,"Price")</f>
-        <v>2042.22</v>
+        <v>2110.6</v>
       </c>
     </row>
     <row r="117" spans="24:25" ht="20" x14ac:dyDescent="0.25">
@@ -11238,7 +11238,7 @@
       </c>
       <c r="Y117" s="53">
         <f>Y115/Y116-1</f>
-        <v>-0.68690150206125711</v>
+        <v>-0.69942764158714188</v>
       </c>
     </row>
     <row r="118" spans="24:25" ht="20" x14ac:dyDescent="0.25">

</xml_diff>